<commit_message>
more OrSplit tests #422
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/TabularActivityBuilderOrSplitDef.xlsx
+++ b/dsl/src/test/data/TabularActivityBuilderOrSplitDef.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0237EC99-5757-4FB0-A96B-2E3C71DE05B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4511AB3D-E594-4F3D-82CB-B35C0639FCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="3015" windowWidth="18900" windowHeight="11115" tabRatio="625" activeTab="3" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" tabRatio="625" activeTab="2" xr2:uid="{A9C7762E-9BDD-441B-8C93-8BFC837C8F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="5" r:id="rId1"/>
     <sheet name="StartWithOrSplit" sheetId="3" r:id="rId2"/>
-    <sheet name="NestedOrSplit" sheetId="6" r:id="rId3"/>
-    <sheet name="OrSplitWithAndSplit" sheetId="7" r:id="rId4"/>
+    <sheet name="SequenceWithOrSplit" sheetId="9" r:id="rId3"/>
+    <sheet name="NestedOrSplit" sheetId="6" r:id="rId4"/>
+    <sheet name="OrSplitWithAndSplit" sheetId="7" r:id="rId5"/>
+    <sheet name="OrSplitWithLoop" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -109,6 +111,24 @@
   </si>
   <si>
     <t>AndRight2</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>LoopRight</t>
+  </si>
+  <si>
+    <t>Left1</t>
+  </si>
+  <si>
+    <t>Left2</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
   </si>
 </sst>
 </file>
@@ -876,6 +896,155 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4208AF-8173-49CE-8202-742E42FDE53A}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5615E36F-9063-4BD8-9022-35D49BED2FCA}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -1019,11 +1188,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2900A3-ADDC-4E07-8A27-81BDC92B4F35}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1161,4 +1330,109 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACFCC7D-C05E-42FE-9363-D787382E6BF7}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>